<commit_message>
Ajuste consumo actualizar proyectos
</commit_message>
<xml_diff>
--- a/docs/Cola_proyectos.xlsx
+++ b/docs/Cola_proyectos.xlsx
@@ -432,17 +432,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="16" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -493,21 +482,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0825-PRUEBA</t>
+          <t>0725-TEST</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>F:\TEST\0825-PRUEBA</t>
+          <t>F:\TEST\0725-TEST</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -515,17 +504,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Completo</t>
+          <t>Sin Dias Rastreos</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CAMILO CASTILLO</t>
+          <t>JEFFERSON BETANCOURT</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">

</xml_diff>